<commit_message>
Unfinished Pinj calc function
</commit_message>
<xml_diff>
--- a/SystemData.xlsx
+++ b/SystemData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/55f28cbac8695f59/Documents/552 Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baumj\OneDrive\Documents\Current Courses\EE 552\552 Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="8_{C3562DA1-6E49-449C-866E-E72AFF8877D4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{F9862B43-34B7-4896-B57D-A5C7236A80D5}"/>
+  <xr:revisionPtr revIDLastSave="122" documentId="8_{C3562DA1-6E49-449C-866E-E72AFF8877D4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{595D088C-9BDB-48FB-A2CD-7F046073D599}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6555" xr2:uid="{E1736FAC-F77A-4764-ABAB-3D17C371FC98}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6555" activeTab="1" xr2:uid="{E1736FAC-F77A-4764-ABAB-3D17C371FC98}"/>
   </bookViews>
   <sheets>
     <sheet name="System Params" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>From Bus</t>
   </si>
@@ -78,9 +78,6 @@
     <t>V</t>
   </si>
   <si>
-    <t>Theta</t>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
@@ -88,6 +85,12 @@
   </si>
   <si>
     <t>H</t>
+  </si>
+  <si>
+    <t>Theta (deg)</t>
+  </si>
+  <si>
+    <t>Theta (rad)</t>
   </si>
 </sst>
 </file>
@@ -441,7 +444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1321520F-227D-4143-AC08-8D19456B6E0F}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -480,7 +483,7 @@
         <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
@@ -709,15 +712,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{761DFDC5-0516-435B-BEF6-25B350A0CBCC}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -725,49 +728,52 @@
         <v>14</v>
       </c>
       <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>1.9991000000000001</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.81340000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0.66610000000000003</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0.2049</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>1.6</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>1.0509999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -777,8 +783,12 @@
       <c r="C5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D5">
+        <f>C5*PI()/180</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -788,8 +798,12 @@
       <c r="C6">
         <v>-3.55</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D6">
+        <f t="shared" ref="D6:D9" si="0">C6*PI()/180</f>
+        <v>-6.1959188445798695E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -799,8 +813,12 @@
       <c r="C7">
         <v>-2.9</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>-5.0614548307835558E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -811,13 +829,17 @@
         <v>-7.48</v>
       </c>
       <c r="D8">
+        <f t="shared" si="0"/>
+        <v>-0.13055062804917586</v>
+      </c>
+      <c r="E8">
         <v>-2.8653</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>-1.2243999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -828,9 +850,13 @@
         <v>-7.05</v>
       </c>
       <c r="D9">
+        <f t="shared" si="0"/>
+        <v>-0.12304571226560024</v>
+      </c>
+      <c r="E9">
         <v>-1.4</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>-0.4</v>
       </c>
     </row>

</xml_diff>